<commit_message>
Update UiDemo_Process.xaml, Update execution timeout to 10 seconds
</commit_message>
<xml_diff>
--- a/Data/Output/Status.xlsx
+++ b/Data/Output/Status.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2A050D-3B5D-49F4-9112-C66CB288E395}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D40D6C0-5482-4BB8-801B-06F14827C407}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,12 +349,14 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C19" sqref="A2:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>